<commit_message>
add 10uF capacitors on VBUS and EN line
</commit_message>
<xml_diff>
--- a/upper-pcb/assembly/BOM.xlsx
+++ b/upper-pcb/assembly/BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gregg\repos\power-meter\upper-pcb\assembly\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B7F6887-1403-4449-AD94-6BCA557339FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DC8C818-A939-4776-AEA8-11FBE6041CF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23136" yWindow="0" windowWidth="23232" windowHeight="13044" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="47160" yWindow="0" windowWidth="23232" windowHeight="26016" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="44">
   <si>
     <t>Comment</t>
   </si>
@@ -83,9 +83,6 @@
     <t>C_33nF_50V_X7R_0603_10</t>
   </si>
   <si>
-    <t>C6_CH1, C6_CH2, C6_CH3, C6_CH4, C10</t>
-  </si>
-  <si>
     <t>C_100nF_50V_X7R_0603_5</t>
   </si>
   <si>
@@ -153,6 +150,21 @@
   </si>
   <si>
     <t>C3011964</t>
+  </si>
+  <si>
+    <t>C6_CH1, C6_CH2, C6_CH3, C6_CH4, C9, C10</t>
+  </si>
+  <si>
+    <t>C_10uF_25V_X7S_0805_10</t>
+  </si>
+  <si>
+    <t>C11, C12</t>
+  </si>
+  <si>
+    <t>C_0805_2012</t>
+  </si>
+  <si>
+    <t>C15850</t>
   </si>
 </sst>
 </file>
@@ -244,8 +256,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{279FC97C-2CC6-4F14-A7AA-D198961FE726}"/>
+    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -600,7 +612,7 @@
   <dimension ref="A1:O48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="19.95" customHeight="1"/>
@@ -643,105 +655,119 @@
         <v>14</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="19.95" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="19.95" customHeight="1">
       <c r="A4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="C4" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="19.95" customHeight="1">
       <c r="A5" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>19</v>
-      </c>
       <c r="D5" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="19.95" customHeight="1">
       <c r="A6" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="D6" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="19.95" customHeight="1">
       <c r="A7" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="19.95" customHeight="1">
       <c r="A8" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="19.95" customHeight="1">
       <c r="A9" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>28</v>
-      </c>
       <c r="D9" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="19.95" customHeight="1">
+      <c r="A10" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:15" ht="19.95" customHeight="1">

</xml_diff>